<commit_message>
Added general path in the artifactsFolder.m script; Included a cast to double in the disturbance output
</commit_message>
<xml_diff>
--- a/SFFS/Simulador/SFF_Simulator_Entradas.xlsx
+++ b/SFFS/Simulador/SFF_Simulator_Entradas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e3e6f638b146f2d7/Mestrado_ITA/Artigos_Certificados/ArtigoFinal2025/SimuladorV2/SFFS/Simulador/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\SFF_Simulator\SFFS\Simulador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{BA22C97C-477C-4762-9136-9048ABF35EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72EFF835-B99F-451B-9942-59ECE4AE3F72}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9506C9C2-880A-43D5-B2A7-AE2A4E62A1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5B485317-3607-4CAD-81D9-5AFA4595F444}"/>
   </bookViews>
@@ -626,10 +626,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1351,10 +1351,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F593E2A8-D4C7-4593-ADB8-821783746406}" name="Tabela1" displayName="Tabela1" ref="B2:D60" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="B2:D60" xr:uid="{F593E2A8-D4C7-4593-ADB8-821783746406}">
@@ -2439,7 +2435,7 @@
   <dimension ref="B2:U45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,16 +2489,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -2517,34 +2513,34 @@
       <c r="U2" s="6"/>
     </row>
     <row r="4" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="E4" s="17" t="s">
+      <c r="C4" s="16"/>
+      <c r="E4" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="H4" s="17" t="s">
+      <c r="F4" s="16"/>
+      <c r="H4" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="K4" s="17" t="s">
+      <c r="I4" s="16"/>
+      <c r="K4" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="17"/>
-      <c r="N4" s="17" t="s">
+      <c r="L4" s="16"/>
+      <c r="N4" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="O4" s="17"/>
-      <c r="Q4" s="17" t="s">
+      <c r="O4" s="16"/>
+      <c r="Q4" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="R4" s="17"/>
-      <c r="T4" s="17" t="s">
+      <c r="R4" s="16"/>
+      <c r="T4" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="U4" s="17"/>
+      <c r="U4" s="16"/>
     </row>
     <row r="5" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -2595,7 +2591,7 @@
         <v>56</v>
       </c>
       <c r="C6" s="1">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>102</v>
@@ -2645,7 +2641,7 @@
         <v>57</v>
       </c>
       <c r="C7" s="4">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>103</v>
@@ -2922,22 +2918,22 @@
       <c r="U15" s="3"/>
     </row>
     <row r="16" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="E16" s="17" t="s">
+      <c r="C16" s="16"/>
+      <c r="E16" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="H16" s="17" t="s">
+      <c r="F16" s="16"/>
+      <c r="H16" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="K16" s="17" t="s">
+      <c r="I16" s="16"/>
+      <c r="K16" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="L16" s="17"/>
+      <c r="L16" s="16"/>
     </row>
     <row r="17" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
@@ -2970,7 +2966,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>32</v>
@@ -3018,7 +3014,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>34</v>
@@ -3040,7 +3036,7 @@
         <v>26</v>
       </c>
       <c r="C21" s="4">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>35</v>
@@ -3084,7 +3080,7 @@
         <v>28</v>
       </c>
       <c r="C23" s="4">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>37</v>
@@ -3106,7 +3102,7 @@
         <v>29</v>
       </c>
       <c r="C24" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -3134,7 +3130,7 @@
         <v>31</v>
       </c>
       <c r="C26" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -3154,24 +3150,24 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="17"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="17" t="s">
+      <c r="H28" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="I28" s="17"/>
-      <c r="K28" s="17" t="s">
+      <c r="I28" s="16"/>
+      <c r="K28" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="L28" s="17"/>
+      <c r="L28" s="16"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
@@ -3554,22 +3550,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K4:L4"/>
     <mergeCell ref="T4:U4"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="N4:O4"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="Q4:R4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>